<commit_message>
Add delete route and update organisation.xlsx
</commit_message>
<xml_diff>
--- a/management/organisation.xlsx
+++ b/management/organisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaseen\Desktop\hometrics\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C66645-1FC6-4FCC-A38B-5C47EFB09B78}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD8BAB5-1245-4E2C-AF0D-E63196AE04B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -304,6 +304,18 @@
   </si>
   <si>
     <t>Migrate database to Heroku PostgreSQL &amp; temperature control backend</t>
+  </si>
+  <si>
+    <t>Complete (except data migration, we are pivoting away from Heroku)</t>
+  </si>
+  <si>
+    <t>1 (excluding data migration work)</t>
+  </si>
+  <si>
+    <t>F-UR 2.2, F-UR 3.10, F-UR 3.11</t>
+  </si>
+  <si>
+    <t>F-UR 2.2, backend of F-UR 3.10 &amp; 3.11, add ActivityIndicator component</t>
   </si>
 </sst>
 </file>
@@ -840,7 +852,18 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1130,17 +1153,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{843EC594-8B61-439A-91A9-B0D87B29EFB0}" name="Table2" displayName="Table2" ref="A1:H7" totalsRowShown="0" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{843EC594-8B61-439A-91A9-B0D87B29EFB0}" name="Table2" displayName="Table2" ref="A1:H7" totalsRowShown="0" dataDxfId="39">
   <autoFilter ref="A1:H7" xr:uid="{0A008C55-1AFE-469E-9B1B-59ECCCBA57E2}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5BDF2CDB-488A-4557-A2F0-16F3BBD2D877}" name="Name" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{804056EB-751D-4FEC-BF8B-AE937D7F5015}" name="Week ending date" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{C6420F38-B6AD-4AF7-845D-1AC7B214087C}" name="Objective" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{5BDF2CDB-488A-4557-A2F0-16F3BBD2D877}" name="Name" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{804056EB-751D-4FEC-BF8B-AE937D7F5015}" name="Week ending date" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{C6420F38-B6AD-4AF7-845D-1AC7B214087C}" name="Objective" dataDxfId="36"/>
     <tableColumn id="9" xr3:uid="{7C3A71D2-7824-43E4-9BC3-4640C1163F66}" name="Satisfactory Progress" dataCellStyle="Good"/>
-    <tableColumn id="4" xr3:uid="{21687B5E-C096-42B5-B358-FF6C453ED4A0}" name="Progress" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{B885D38E-90CB-4675-9A13-6C8DD7B84851}" name="Deliverables" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{1EE46279-20F5-436E-A029-B70FEDE1349C}" name="Dependencies" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{B04E38F6-8793-49E9-A252-04A2A1A35EDC}" name="Hours" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{21687B5E-C096-42B5-B358-FF6C453ED4A0}" name="Progress" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{B885D38E-90CB-4675-9A13-6C8DD7B84851}" name="Deliverables" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{1EE46279-20F5-436E-A029-B70FEDE1349C}" name="Dependencies" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{B04E38F6-8793-49E9-A252-04A2A1A35EDC}" name="Hours" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1151,9 +1174,9 @@
   <autoFilter ref="A73:H79" xr:uid="{D8F26B56-D129-42DB-B906-ECC3FD9D98AC}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E7958848-6E54-42D8-8015-31182E5D7B27}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{E7CE1CB3-CCE5-4077-9B08-488BCB1D9EF4}" name="Week ending date" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E7CE1CB3-CCE5-4077-9B08-488BCB1D9EF4}" name="Week ending date" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{4D9FAB89-789D-4671-A910-86A17409EA96}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{475CFC22-1905-4BBA-9844-372E63A07AFE}" name="Satisfactory Progress" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{475CFC22-1905-4BBA-9844-372E63A07AFE}" name="Satisfactory Progress" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{DB346AA5-986D-451A-B8D9-8A3AD26B046C}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{AA7F919D-2842-4ADE-A599-6E4452C1E440}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{D70A771E-6948-4BBD-9EE8-FC159BA62161}" name="Dependencies"/>
@@ -1168,9 +1191,9 @@
   <autoFilter ref="A81:H87" xr:uid="{15E8E00F-0F44-4534-AAF0-D8548D329B9F}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B103AC18-C508-429B-A263-B7B31A783B0F}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{FA545805-1077-4FF3-BC3A-C6CBA99D35D5}" name="Week ending date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FA545805-1077-4FF3-BC3A-C6CBA99D35D5}" name="Week ending date" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{DC87C481-39A1-4D17-9674-D072F67C35E9}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{55757F20-3C60-45D1-830A-12DCAA6EA793}" name="Satisfactory Progress" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{55757F20-3C60-45D1-830A-12DCAA6EA793}" name="Satisfactory Progress" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{E351D832-0001-4863-910F-4BB23F082B12}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{83A49415-8729-4623-A4D2-03EDB218FB0E}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{2B78A1B0-88DC-4B9E-B068-3BB6976D9311}" name="Dependencies"/>
@@ -1185,9 +1208,9 @@
   <autoFilter ref="A89:H95" xr:uid="{2ECDB29E-3D42-4AD4-87A9-8823F17D02AD}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0B3E0BF7-204D-4FED-820B-A1C91D9E6F73}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{45E346E3-AF50-4000-B5EF-A171F59A05E7}" name="Week ending date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{45E346E3-AF50-4000-B5EF-A171F59A05E7}" name="Week ending date" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{DC34F243-8204-415E-B7F8-4802E219F8D1}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{049E9916-4A23-4061-B56D-3ED23F749CBB}" name="Satisfactory Progress" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{049E9916-4A23-4061-B56D-3ED23F749CBB}" name="Satisfactory Progress" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{0C233A8F-B9B1-43A5-A3A0-0C19F6236C1E}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{FAB75192-B753-42D9-AD12-AEAFCB43131D}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{47BCB8E7-4CBF-49DD-A2D1-88919DA0EA1C}" name="Dependencies"/>
@@ -1202,13 +1225,30 @@
   <autoFilter ref="A97:H103" xr:uid="{A98912C6-4862-4588-B977-85807101FA59}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3948D17F-1168-4CF6-923C-2C77219C37D3}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{12C76E18-2BBB-49A3-BEC4-42902DE30713}" name="Week ending date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{12C76E18-2BBB-49A3-BEC4-42902DE30713}" name="Week ending date" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{E960D0C1-0514-4352-9DD5-7B303BFB2219}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{5B33989F-43AD-4C48-9BD7-47CFE84BC06D}" name="Satisfactory Progress" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{5B33989F-43AD-4C48-9BD7-47CFE84BC06D}" name="Satisfactory Progress" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{9F4A9C8D-999D-43C2-B5AE-F4D51F04346A}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{DB987D03-A94E-450E-9E75-384DA948ED82}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{ED65F018-A973-4B37-87D3-702B6075CF4D}" name="Dependencies"/>
     <tableColumn id="7" xr3:uid="{A4D0A9B2-1AB5-404A-B5B0-77D9A5C808E4}" name="Hours"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FB284D11-F3FC-4EB7-A812-757A6602F1AF}" name="Table327689101112131415" displayName="Table327689101112131415" ref="A105:H111" totalsRowShown="0">
+  <autoFilter ref="A105:H111" xr:uid="{04FCD7BA-51FA-4800-AAF5-459728AEB57E}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{233CFB38-7434-4F67-A968-2C8F7834ADA3}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{16C30C02-B555-4C2C-AFEF-93D4250E70C9}" name="Week ending date" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{12C53416-BB78-4AF7-BA13-E888C4298890}" name="Objective"/>
+    <tableColumn id="8" xr3:uid="{DC8573AA-BC56-45E0-9A85-F2935A69A715}" name="Satisfactory Progress" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{A46BB867-8D55-4478-AD3F-E589CE9DAC96}" name="Progress"/>
+    <tableColumn id="5" xr3:uid="{E23945B5-072A-466E-8667-C3060781B387}" name="Deliverables"/>
+    <tableColumn id="6" xr3:uid="{2CAE5519-C476-4F22-A928-71031C96FE75}" name="Dependencies"/>
+    <tableColumn id="7" xr3:uid="{12BB5AD2-7B18-48F3-BBC7-A43CA4FAD6F3}" name="Hours"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1219,7 +1259,7 @@
   <autoFilter ref="A9:H15" xr:uid="{9B15872F-D7B6-401E-831C-28C7BB633115}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C13B2CF4-3F76-4D51-B756-D111A72296FB}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{957E14F0-6710-4907-A5C5-D6E5AC31AA5D}" name="Week ending date" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{957E14F0-6710-4907-A5C5-D6E5AC31AA5D}" name="Week ending date" dataDxfId="31"/>
     <tableColumn id="3" xr3:uid="{77D7746D-18EF-4BA5-B8F5-B743F6E15B4E}" name="Objective"/>
     <tableColumn id="8" xr3:uid="{EF91DA4F-CBB3-4C2E-BE11-3FF42E040801}" name="Satisfactory Progress" dataCellStyle="Good"/>
     <tableColumn id="4" xr3:uid="{93A5D790-2610-40CF-822C-0C84A09B6FE8}" name="Progress"/>
@@ -1232,17 +1272,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FD7340E-182D-43F5-938D-6092047D1063}" name="Table32" displayName="Table32" ref="A17:H23" totalsRowShown="0" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FD7340E-182D-43F5-938D-6092047D1063}" name="Table32" displayName="Table32" ref="A17:H23" totalsRowShown="0" dataDxfId="30">
   <autoFilter ref="A17:H23" xr:uid="{AF172F78-D62B-4280-84ED-8C6B5ACDF354}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F3BD302C-C92C-4942-BD36-FA304D64F3EB}" name="Name" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{5DDBB7FD-4EE8-4F7E-A3D2-6B5A752631DF}" name="Week ending date" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{EF127786-A680-4211-B5BF-6661403383A6}" name="Objective" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{7218DB10-0B84-434B-A19F-BECFC273CDFA}" name="Satisfactory Progress" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{CBDBB2B4-ED80-4195-9D9F-B052AA6F1BAB}" name="Progress" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{0AA61E4B-0301-4C64-94A1-EA6DF7F98D6A}" name="Deliverables" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{DE9AF41C-DA93-41F7-8B94-CB8CABB0A48C}" name="Dependencies" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{53B9A5C7-49FF-497D-A8B8-1C8A6867F726}" name="Hours" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{F3BD302C-C92C-4942-BD36-FA304D64F3EB}" name="Name" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{5DDBB7FD-4EE8-4F7E-A3D2-6B5A752631DF}" name="Week ending date" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{EF127786-A680-4211-B5BF-6661403383A6}" name="Objective" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{7218DB10-0B84-434B-A19F-BECFC273CDFA}" name="Satisfactory Progress" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{CBDBB2B4-ED80-4195-9D9F-B052AA6F1BAB}" name="Progress" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{0AA61E4B-0301-4C64-94A1-EA6DF7F98D6A}" name="Deliverables" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{DE9AF41C-DA93-41F7-8B94-CB8CABB0A48C}" name="Dependencies" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{53B9A5C7-49FF-497D-A8B8-1C8A6867F726}" name="Hours" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1253,9 +1293,9 @@
   <autoFilter ref="A33:H39" xr:uid="{0A54035B-5321-4F41-8018-2E72ABE1A3CE}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7EB17E51-19DB-472E-8181-6DB89BD35F8A}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{9F725E84-51E8-4EE6-AE33-BD3341C0933D}" name="Week ending date" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{9F725E84-51E8-4EE6-AE33-BD3341C0933D}" name="Week ending date" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{63C2F6D4-86F2-47E9-AAD5-955ACF3E8861}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{295EF8C6-9C55-4347-844E-A4A75F81AC1F}" name="Satisfactory Progress" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{295EF8C6-9C55-4347-844E-A4A75F81AC1F}" name="Satisfactory Progress" dataDxfId="20"/>
     <tableColumn id="4" xr3:uid="{F5A99744-24AA-4B13-BB4F-EFD4E6BF40FD}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{B39838FB-0086-4A72-9E14-C0C5B3F4F9AD}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{CF988054-5385-4AEB-B9E6-4C0F08E7DA75}" name="Dependencies"/>
@@ -1270,9 +1310,9 @@
   <autoFilter ref="A25:H31" xr:uid="{DA227A29-4C8A-4B67-9C8E-01733A0B3317}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F0850E0F-9829-4438-8D05-D79BBC233B1C}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{3B2351F9-F706-4D7A-BB34-513C649561F8}" name="Week ending date" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{3B2351F9-F706-4D7A-BB34-513C649561F8}" name="Week ending date" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{B476097B-479E-43CD-8911-FA9155FA6DBF}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{9B1BC001-E56D-4DF0-8CF5-3B5133733D4C}" name="Satisfactory Progress" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{9B1BC001-E56D-4DF0-8CF5-3B5133733D4C}" name="Satisfactory Progress" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{F5B94650-8D72-4165-AB08-C77CF5DC0089}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{853EA2D7-46E8-488E-A974-5EEEF25BE38A}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{5BE041A0-A5A6-4889-816E-965200BC15AE}" name="Dependencies"/>
@@ -1287,9 +1327,9 @@
   <autoFilter ref="A41:H47" xr:uid="{D2FBF5FD-E02E-40E7-8E34-C484653BF6DF}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{779B12E3-CF8D-4362-8564-A04744DFE317}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{72623AFD-AE5D-472D-BA2D-325EDEC3BBC8}" name="Week ending date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{72623AFD-AE5D-472D-BA2D-325EDEC3BBC8}" name="Week ending date" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{4E1545E5-A24C-4965-809E-8D5324CA29E0}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{233D036F-651C-4121-A865-8F7079B3F8B0}" name="Satisfactory Progress" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{233D036F-651C-4121-A865-8F7079B3F8B0}" name="Satisfactory Progress" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{27455D0B-2536-476E-A2E7-089B51EE8641}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{FDE0141F-DFB7-407A-AE25-E0F13041EDC8}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{00D62C56-F25E-406A-B0F0-E9E69B6E1BD3}" name="Dependencies"/>
@@ -1304,9 +1344,9 @@
   <autoFilter ref="A49:H55" xr:uid="{B907C122-58AE-44A3-9818-AFAFCE2F4740}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{90506F9F-7541-496A-A43C-7FD7EC833D65}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{142A1AC6-E52C-4274-A965-776324EF804D}" name="Week ending date" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{142A1AC6-E52C-4274-A965-776324EF804D}" name="Week ending date" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{EE832172-8D63-453D-83A9-2DFD9679AB1E}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{F334C323-90CA-4279-B12A-94F3D8479154}" name="Satisfactory Progress" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{F334C323-90CA-4279-B12A-94F3D8479154}" name="Satisfactory Progress" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{9460083D-A7ED-4816-ADDE-8D94BBCAE2DA}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{E1713EE3-5356-4486-9FA6-43D6515C6185}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{A6623A90-3F9C-4346-A84B-C32025CC31B8}" name="Dependencies"/>
@@ -1321,9 +1361,9 @@
   <autoFilter ref="A57:H63" xr:uid="{5EAA595B-BCCD-4CC6-8C37-C37A62376111}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C3C8235C-CFD2-4419-922F-81C9263AC468}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{3EA2B805-841C-46B6-AA87-0255A0B19F40}" name="Week ending date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3EA2B805-841C-46B6-AA87-0255A0B19F40}" name="Week ending date" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{7038F8A8-6518-4B57-A98C-328098C84ACF}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{19202101-9DC4-4AB1-AE91-3D0165543914}" name="Satisfactory Progress" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{19202101-9DC4-4AB1-AE91-3D0165543914}" name="Satisfactory Progress" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{B60F6342-2420-4464-9FE1-640027DFFA28}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{82C08185-62B0-49B8-8BF8-A43FAD604047}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{CAD1A98A-74B0-4F1D-ADD6-0C436D5EDB8E}" name="Dependencies"/>
@@ -1338,9 +1378,9 @@
   <autoFilter ref="A65:H71" xr:uid="{94928A84-CEC8-4686-A48A-A106421EFF97}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{122D3763-DD48-4DB8-8D44-5D63ED13E699}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{FCD2BFCD-EF2B-4360-B3AE-7271D88EC80B}" name="Week ending date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{FCD2BFCD-EF2B-4360-B3AE-7271D88EC80B}" name="Week ending date" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{BC0C5139-381F-421E-82A5-8F2665A6D53A}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{27E0CB91-7760-4BBE-98CF-37C7F0809D4C}" name="Satisfactory Progress" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{27E0CB91-7760-4BBE-98CF-37C7F0809D4C}" name="Satisfactory Progress" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{9BFB9637-598D-41DD-B2F0-A8C74A76ABAE}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{C0CAB8E0-A4F5-4C92-8BC8-BDFAC6FC58B3}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{8C5A0E92-FB26-4C7B-B09F-68CCE093EF0B}" name="Dependencies"/>
@@ -1647,20 +1687,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="55.77734375" customWidth="1"/>
+    <col min="3" max="3" width="57.44140625" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="6" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
     <col min="7" max="7" width="38.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -3924,29 +3966,29 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="A100" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="4">
         <v>43888</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G100" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E100" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F100" t="s">
-        <v>75</v>
-      </c>
-      <c r="G100" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H100" s="5" t="s">
-        <v>63</v>
+      <c r="H100" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
@@ -4024,6 +4066,170 @@
         <v>12</v>
       </c>
       <c r="H103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
+        <v>3</v>
+      </c>
+      <c r="E105" t="s">
+        <v>4</v>
+      </c>
+      <c r="F105" t="s">
+        <v>5</v>
+      </c>
+      <c r="G105" t="s">
+        <v>6</v>
+      </c>
+      <c r="H105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>50</v>
+      </c>
+      <c r="B106" s="6"/>
+      <c r="C106" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>51</v>
+      </c>
+      <c r="B107" s="6"/>
+      <c r="C107" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B108" s="4">
+        <v>43895</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H108" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>53</v>
+      </c>
+      <c r="B109" s="6"/>
+      <c r="C109" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B110" s="2">
+        <v>43888</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B111" s="2">
+        <v>43888</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H111" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4040,7 +4246,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
-  <tableParts count="13">
+  <tableParts count="14">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -4054,6 +4260,7 @@
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Settings Screen + fixes
Fixed energy screen layout, added setting screen skeleton and updated organisation
</commit_message>
<xml_diff>
--- a/management/organisation.xlsx
+++ b/management/organisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaseen\Desktop\hometrics\management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tzevi\OneDrive\Documents\GitHub\hometrics\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD8BAB5-1245-4E2C-AF0D-E63196AE04B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{BBD8BAB5-1245-4E2C-AF0D-E63196AE04B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{316563CC-8DE3-4D1C-8DCC-DFE8E26DD8E6}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>F-UR 2.2, backend of F-UR 3.10 &amp; 3.11, add ActivityIndicator component</t>
+  </si>
+  <si>
+    <t>Settings Page</t>
   </si>
 </sst>
 </file>
@@ -1690,22 +1693,22 @@
   <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="57.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="55.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="7" width="38.44140625" customWidth="1"/>
-    <col min="8" max="8" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.52734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.41015625" customWidth="1"/>
+    <col min="3" max="3" width="57.41015625" customWidth="1"/>
+    <col min="4" max="4" width="19.64453125" customWidth="1"/>
+    <col min="5" max="5" width="55.64453125" customWidth="1"/>
+    <col min="6" max="6" width="25.87890625" customWidth="1"/>
+    <col min="7" max="7" width="38.41015625" customWidth="1"/>
+    <col min="8" max="8" width="27.76171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>51</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -1809,7 +1812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -2043,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -2147,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
@@ -2199,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
@@ -2225,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -2303,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
@@ -2329,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -2355,7 +2358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
@@ -2433,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="s">
         <v>51</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="s">
         <v>52</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="s">
         <v>53</v>
       </c>
@@ -2563,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="s">
         <v>54</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="s">
         <v>50</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A43" s="3" t="s">
         <v>51</v>
       </c>
@@ -2693,7 +2696,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="s">
         <v>52</v>
       </c>
@@ -2719,7 +2722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
@@ -2745,7 +2748,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A46" s="3" t="s">
         <v>54</v>
       </c>
@@ -2771,7 +2774,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -2795,7 +2798,7 @@
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
@@ -2847,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
@@ -2873,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A52" s="3" t="s">
         <v>52</v>
       </c>
@@ -2899,7 +2902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A53" s="3" t="s">
         <v>53</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
@@ -2951,7 +2954,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -3003,7 +3006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A58" s="3" t="s">
         <v>50</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A59" s="3" t="s">
         <v>51</v>
       </c>
@@ -3055,7 +3058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A60" s="3" t="s">
         <v>52</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A61" s="3" t="s">
         <v>53</v>
       </c>
@@ -3107,7 +3110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
@@ -3133,7 +3136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
@@ -3159,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -3185,7 +3188,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A66" s="3" t="s">
         <v>50</v>
       </c>
@@ -3211,7 +3214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A67" s="3" t="s">
         <v>51</v>
       </c>
@@ -3237,7 +3240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A68" s="3" t="s">
         <v>52</v>
       </c>
@@ -3263,7 +3266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A69" s="3" t="s">
         <v>53</v>
       </c>
@@ -3289,7 +3292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
         <v>54</v>
       </c>
@@ -3315,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>55</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -3367,7 +3370,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A74" s="3" t="s">
         <v>50</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A75" s="3" t="s">
         <v>51</v>
       </c>
@@ -3419,7 +3422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A76" s="3" t="s">
         <v>52</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A77" s="3" t="s">
         <v>53</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
         <v>54</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>55</v>
       </c>
@@ -3523,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -3549,7 +3552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A82" s="3" t="s">
         <v>50</v>
       </c>
@@ -3575,7 +3578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A83" s="3" t="s">
         <v>51</v>
       </c>
@@ -3601,7 +3604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A84" s="3" t="s">
         <v>52</v>
       </c>
@@ -3627,7 +3630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A85" s="3" t="s">
         <v>53</v>
       </c>
@@ -3653,7 +3656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
         <v>54</v>
       </c>
@@ -3679,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
         <v>55</v>
       </c>
@@ -3705,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -3731,7 +3734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A90" s="3" t="s">
         <v>50</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A91" s="3" t="s">
         <v>51</v>
       </c>
@@ -3783,7 +3786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A92" s="3" t="s">
         <v>52</v>
       </c>
@@ -3809,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A93" s="3" t="s">
         <v>53</v>
       </c>
@@ -3835,7 +3838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
         <v>54</v>
       </c>
@@ -3861,7 +3864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
         <v>55</v>
       </c>
@@ -3887,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -3913,7 +3916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A98" t="s">
         <v>50</v>
       </c>
@@ -3939,33 +3942,33 @@
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A99" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="4">
         <v>43888</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D99" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="D99" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G99" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H99" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G99" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H99" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A100" s="3" t="s">
         <v>52</v>
       </c>
@@ -3991,7 +3994,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A101" t="s">
         <v>53</v>
       </c>
@@ -4017,7 +4020,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
         <v>54</v>
       </c>
@@ -4043,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
         <v>55</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -4095,7 +4098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -4115,13 +4118,15 @@
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A107" t="s">
         <v>51</v>
       </c>
-      <c r="B107" s="6"/>
+      <c r="B107" s="6">
+        <v>43895</v>
+      </c>
       <c r="C107" s="5" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>63</v>
@@ -4135,7 +4140,7 @@
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A108" s="3" t="s">
         <v>52</v>
       </c>
@@ -4161,7 +4166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A109" t="s">
         <v>53</v>
       </c>
@@ -4181,7 +4186,7 @@
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
         <v>54</v>
       </c>
@@ -4207,7 +4212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Please fill in the spreadsheet, everybody
</commit_message>
<xml_diff>
--- a/management/organisation.xlsx
+++ b/management/organisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tzevi\OneDrive\Documents\GitHub\hometrics\management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaseen\Desktop\hometrics\management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{BBD8BAB5-1245-4E2C-AF0D-E63196AE04B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{316563CC-8DE3-4D1C-8DCC-DFE8E26DD8E6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992ACDE8-77CE-44E2-A961-FC7C928553BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t>Settings Page</t>
+  </si>
+  <si>
+    <t>Complete backend (except Lee's assignment), Complete frontend with Vincent</t>
+  </si>
+  <si>
+    <t>UI, Backend</t>
   </si>
 </sst>
 </file>
@@ -855,7 +861,18 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1156,17 +1173,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{843EC594-8B61-439A-91A9-B0D87B29EFB0}" name="Table2" displayName="Table2" ref="A1:H7" totalsRowShown="0" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{843EC594-8B61-439A-91A9-B0D87B29EFB0}" name="Table2" displayName="Table2" ref="A1:H7" totalsRowShown="0" dataDxfId="41">
   <autoFilter ref="A1:H7" xr:uid="{0A008C55-1AFE-469E-9B1B-59ECCCBA57E2}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5BDF2CDB-488A-4557-A2F0-16F3BBD2D877}" name="Name" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{804056EB-751D-4FEC-BF8B-AE937D7F5015}" name="Week ending date" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{C6420F38-B6AD-4AF7-845D-1AC7B214087C}" name="Objective" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{5BDF2CDB-488A-4557-A2F0-16F3BBD2D877}" name="Name" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{804056EB-751D-4FEC-BF8B-AE937D7F5015}" name="Week ending date" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{C6420F38-B6AD-4AF7-845D-1AC7B214087C}" name="Objective" dataDxfId="38"/>
     <tableColumn id="9" xr3:uid="{7C3A71D2-7824-43E4-9BC3-4640C1163F66}" name="Satisfactory Progress" dataCellStyle="Good"/>
-    <tableColumn id="4" xr3:uid="{21687B5E-C096-42B5-B358-FF6C453ED4A0}" name="Progress" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{B885D38E-90CB-4675-9A13-6C8DD7B84851}" name="Deliverables" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{1EE46279-20F5-436E-A029-B70FEDE1349C}" name="Dependencies" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{B04E38F6-8793-49E9-A252-04A2A1A35EDC}" name="Hours" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{21687B5E-C096-42B5-B358-FF6C453ED4A0}" name="Progress" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{B885D38E-90CB-4675-9A13-6C8DD7B84851}" name="Deliverables" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{1EE46279-20F5-436E-A029-B70FEDE1349C}" name="Dependencies" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{B04E38F6-8793-49E9-A252-04A2A1A35EDC}" name="Hours" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1177,9 +1194,9 @@
   <autoFilter ref="A73:H79" xr:uid="{D8F26B56-D129-42DB-B906-ECC3FD9D98AC}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E7958848-6E54-42D8-8015-31182E5D7B27}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{E7CE1CB3-CCE5-4077-9B08-488BCB1D9EF4}" name="Week ending date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{E7CE1CB3-CCE5-4077-9B08-488BCB1D9EF4}" name="Week ending date" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{4D9FAB89-789D-4671-A910-86A17409EA96}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{475CFC22-1905-4BBA-9844-372E63A07AFE}" name="Satisfactory Progress" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{475CFC22-1905-4BBA-9844-372E63A07AFE}" name="Satisfactory Progress" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{DB346AA5-986D-451A-B8D9-8A3AD26B046C}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{AA7F919D-2842-4ADE-A599-6E4452C1E440}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{D70A771E-6948-4BBD-9EE8-FC159BA62161}" name="Dependencies"/>
@@ -1194,9 +1211,9 @@
   <autoFilter ref="A81:H87" xr:uid="{15E8E00F-0F44-4534-AAF0-D8548D329B9F}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B103AC18-C508-429B-A263-B7B31A783B0F}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{FA545805-1077-4FF3-BC3A-C6CBA99D35D5}" name="Week ending date" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{FA545805-1077-4FF3-BC3A-C6CBA99D35D5}" name="Week ending date" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{DC87C481-39A1-4D17-9674-D072F67C35E9}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{55757F20-3C60-45D1-830A-12DCAA6EA793}" name="Satisfactory Progress" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{55757F20-3C60-45D1-830A-12DCAA6EA793}" name="Satisfactory Progress" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{E351D832-0001-4863-910F-4BB23F082B12}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{83A49415-8729-4623-A4D2-03EDB218FB0E}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{2B78A1B0-88DC-4B9E-B068-3BB6976D9311}" name="Dependencies"/>
@@ -1211,9 +1228,9 @@
   <autoFilter ref="A89:H95" xr:uid="{2ECDB29E-3D42-4AD4-87A9-8823F17D02AD}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0B3E0BF7-204D-4FED-820B-A1C91D9E6F73}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{45E346E3-AF50-4000-B5EF-A171F59A05E7}" name="Week ending date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{45E346E3-AF50-4000-B5EF-A171F59A05E7}" name="Week ending date" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{DC34F243-8204-415E-B7F8-4802E219F8D1}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{049E9916-4A23-4061-B56D-3ED23F749CBB}" name="Satisfactory Progress" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{049E9916-4A23-4061-B56D-3ED23F749CBB}" name="Satisfactory Progress" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{0C233A8F-B9B1-43A5-A3A0-0C19F6236C1E}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{FAB75192-B753-42D9-AD12-AEAFCB43131D}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{47BCB8E7-4CBF-49DD-A2D1-88919DA0EA1C}" name="Dependencies"/>
@@ -1228,9 +1245,9 @@
   <autoFilter ref="A97:H103" xr:uid="{A98912C6-4862-4588-B977-85807101FA59}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3948D17F-1168-4CF6-923C-2C77219C37D3}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{12C76E18-2BBB-49A3-BEC4-42902DE30713}" name="Week ending date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{12C76E18-2BBB-49A3-BEC4-42902DE30713}" name="Week ending date" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{E960D0C1-0514-4352-9DD5-7B303BFB2219}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{5B33989F-43AD-4C48-9BD7-47CFE84BC06D}" name="Satisfactory Progress" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{5B33989F-43AD-4C48-9BD7-47CFE84BC06D}" name="Satisfactory Progress" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{9F4A9C8D-999D-43C2-B5AE-F4D51F04346A}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{DB987D03-A94E-450E-9E75-384DA948ED82}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{ED65F018-A973-4B37-87D3-702B6075CF4D}" name="Dependencies"/>
@@ -1245,13 +1262,30 @@
   <autoFilter ref="A105:H111" xr:uid="{04FCD7BA-51FA-4800-AAF5-459728AEB57E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{233CFB38-7434-4F67-A968-2C8F7834ADA3}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{16C30C02-B555-4C2C-AFEF-93D4250E70C9}" name="Week ending date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{16C30C02-B555-4C2C-AFEF-93D4250E70C9}" name="Week ending date" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{12C53416-BB78-4AF7-BA13-E888C4298890}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{DC8573AA-BC56-45E0-9A85-F2935A69A715}" name="Satisfactory Progress" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{DC8573AA-BC56-45E0-9A85-F2935A69A715}" name="Satisfactory Progress" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{A46BB867-8D55-4478-AD3F-E589CE9DAC96}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{E23945B5-072A-466E-8667-C3060781B387}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{2CAE5519-C476-4F22-A928-71031C96FE75}" name="Dependencies"/>
     <tableColumn id="7" xr3:uid="{12BB5AD2-7B18-48F3-BBC7-A43CA4FAD6F3}" name="Hours"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{FC1BD2C4-12F3-47C1-A1C0-38E4CDCC5686}" name="Table32768910111213141517" displayName="Table32768910111213141517" ref="A113:H119" totalsRowShown="0">
+  <autoFilter ref="A113:H119" xr:uid="{8E894E41-39B1-47AA-9E6D-5E9586182F01}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{13833338-C426-4D92-8AD3-73C86EA4C514}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{B0609326-C0C9-4F93-B68D-85858AB867B1}" name="Week ending date" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{83BEAA31-CF71-4A41-BB37-3C59E8F08725}" name="Objective"/>
+    <tableColumn id="8" xr3:uid="{530E79A0-6CE6-446B-8903-9CBF0E4860E9}" name="Satisfactory Progress" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{4A1D7770-A655-451B-AD19-4407A3168A89}" name="Progress"/>
+    <tableColumn id="5" xr3:uid="{7372B397-F7A4-4A85-9C62-56475FADBF1C}" name="Deliverables"/>
+    <tableColumn id="6" xr3:uid="{C61A999B-7D38-43C5-BAE2-C91480C97E6A}" name="Dependencies"/>
+    <tableColumn id="7" xr3:uid="{7567FCDC-7111-4D3B-8CBB-E57A218C5A60}" name="Hours"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1262,7 +1296,7 @@
   <autoFilter ref="A9:H15" xr:uid="{9B15872F-D7B6-401E-831C-28C7BB633115}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C13B2CF4-3F76-4D51-B756-D111A72296FB}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{957E14F0-6710-4907-A5C5-D6E5AC31AA5D}" name="Week ending date" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{957E14F0-6710-4907-A5C5-D6E5AC31AA5D}" name="Week ending date" dataDxfId="33"/>
     <tableColumn id="3" xr3:uid="{77D7746D-18EF-4BA5-B8F5-B743F6E15B4E}" name="Objective"/>
     <tableColumn id="8" xr3:uid="{EF91DA4F-CBB3-4C2E-BE11-3FF42E040801}" name="Satisfactory Progress" dataCellStyle="Good"/>
     <tableColumn id="4" xr3:uid="{93A5D790-2610-40CF-822C-0C84A09B6FE8}" name="Progress"/>
@@ -1275,17 +1309,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FD7340E-182D-43F5-938D-6092047D1063}" name="Table32" displayName="Table32" ref="A17:H23" totalsRowShown="0" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FD7340E-182D-43F5-938D-6092047D1063}" name="Table32" displayName="Table32" ref="A17:H23" totalsRowShown="0" dataDxfId="32">
   <autoFilter ref="A17:H23" xr:uid="{AF172F78-D62B-4280-84ED-8C6B5ACDF354}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F3BD302C-C92C-4942-BD36-FA304D64F3EB}" name="Name" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{5DDBB7FD-4EE8-4F7E-A3D2-6B5A752631DF}" name="Week ending date" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{EF127786-A680-4211-B5BF-6661403383A6}" name="Objective" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{7218DB10-0B84-434B-A19F-BECFC273CDFA}" name="Satisfactory Progress" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{CBDBB2B4-ED80-4195-9D9F-B052AA6F1BAB}" name="Progress" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{0AA61E4B-0301-4C64-94A1-EA6DF7F98D6A}" name="Deliverables" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{DE9AF41C-DA93-41F7-8B94-CB8CABB0A48C}" name="Dependencies" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{53B9A5C7-49FF-497D-A8B8-1C8A6867F726}" name="Hours" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{F3BD302C-C92C-4942-BD36-FA304D64F3EB}" name="Name" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{5DDBB7FD-4EE8-4F7E-A3D2-6B5A752631DF}" name="Week ending date" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{EF127786-A680-4211-B5BF-6661403383A6}" name="Objective" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{7218DB10-0B84-434B-A19F-BECFC273CDFA}" name="Satisfactory Progress" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{CBDBB2B4-ED80-4195-9D9F-B052AA6F1BAB}" name="Progress" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{0AA61E4B-0301-4C64-94A1-EA6DF7F98D6A}" name="Deliverables" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{DE9AF41C-DA93-41F7-8B94-CB8CABB0A48C}" name="Dependencies" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{53B9A5C7-49FF-497D-A8B8-1C8A6867F726}" name="Hours" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1296,9 +1330,9 @@
   <autoFilter ref="A33:H39" xr:uid="{0A54035B-5321-4F41-8018-2E72ABE1A3CE}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7EB17E51-19DB-472E-8181-6DB89BD35F8A}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{9F725E84-51E8-4EE6-AE33-BD3341C0933D}" name="Week ending date" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{9F725E84-51E8-4EE6-AE33-BD3341C0933D}" name="Week ending date" dataDxfId="23"/>
     <tableColumn id="3" xr3:uid="{63C2F6D4-86F2-47E9-AAD5-955ACF3E8861}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{295EF8C6-9C55-4347-844E-A4A75F81AC1F}" name="Satisfactory Progress" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{295EF8C6-9C55-4347-844E-A4A75F81AC1F}" name="Satisfactory Progress" dataDxfId="22"/>
     <tableColumn id="4" xr3:uid="{F5A99744-24AA-4B13-BB4F-EFD4E6BF40FD}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{B39838FB-0086-4A72-9E14-C0C5B3F4F9AD}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{CF988054-5385-4AEB-B9E6-4C0F08E7DA75}" name="Dependencies"/>
@@ -1313,9 +1347,9 @@
   <autoFilter ref="A25:H31" xr:uid="{DA227A29-4C8A-4B67-9C8E-01733A0B3317}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F0850E0F-9829-4438-8D05-D79BBC233B1C}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{3B2351F9-F706-4D7A-BB34-513C649561F8}" name="Week ending date" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{3B2351F9-F706-4D7A-BB34-513C649561F8}" name="Week ending date" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{B476097B-479E-43CD-8911-FA9155FA6DBF}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{9B1BC001-E56D-4DF0-8CF5-3B5133733D4C}" name="Satisfactory Progress" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{9B1BC001-E56D-4DF0-8CF5-3B5133733D4C}" name="Satisfactory Progress" dataDxfId="20"/>
     <tableColumn id="4" xr3:uid="{F5B94650-8D72-4165-AB08-C77CF5DC0089}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{853EA2D7-46E8-488E-A974-5EEEF25BE38A}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{5BE041A0-A5A6-4889-816E-965200BC15AE}" name="Dependencies"/>
@@ -1330,9 +1364,9 @@
   <autoFilter ref="A41:H47" xr:uid="{D2FBF5FD-E02E-40E7-8E34-C484653BF6DF}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{779B12E3-CF8D-4362-8564-A04744DFE317}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{72623AFD-AE5D-472D-BA2D-325EDEC3BBC8}" name="Week ending date" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{72623AFD-AE5D-472D-BA2D-325EDEC3BBC8}" name="Week ending date" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{4E1545E5-A24C-4965-809E-8D5324CA29E0}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{233D036F-651C-4121-A865-8F7079B3F8B0}" name="Satisfactory Progress" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{233D036F-651C-4121-A865-8F7079B3F8B0}" name="Satisfactory Progress" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{27455D0B-2536-476E-A2E7-089B51EE8641}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{FDE0141F-DFB7-407A-AE25-E0F13041EDC8}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{00D62C56-F25E-406A-B0F0-E9E69B6E1BD3}" name="Dependencies"/>
@@ -1347,9 +1381,9 @@
   <autoFilter ref="A49:H55" xr:uid="{B907C122-58AE-44A3-9818-AFAFCE2F4740}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{90506F9F-7541-496A-A43C-7FD7EC833D65}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{142A1AC6-E52C-4274-A965-776324EF804D}" name="Week ending date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{142A1AC6-E52C-4274-A965-776324EF804D}" name="Week ending date" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{EE832172-8D63-453D-83A9-2DFD9679AB1E}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{F334C323-90CA-4279-B12A-94F3D8479154}" name="Satisfactory Progress" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{F334C323-90CA-4279-B12A-94F3D8479154}" name="Satisfactory Progress" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{9460083D-A7ED-4816-ADDE-8D94BBCAE2DA}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{E1713EE3-5356-4486-9FA6-43D6515C6185}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{A6623A90-3F9C-4346-A84B-C32025CC31B8}" name="Dependencies"/>
@@ -1364,9 +1398,9 @@
   <autoFilter ref="A57:H63" xr:uid="{5EAA595B-BCCD-4CC6-8C37-C37A62376111}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C3C8235C-CFD2-4419-922F-81C9263AC468}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{3EA2B805-841C-46B6-AA87-0255A0B19F40}" name="Week ending date" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{3EA2B805-841C-46B6-AA87-0255A0B19F40}" name="Week ending date" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{7038F8A8-6518-4B57-A98C-328098C84ACF}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{19202101-9DC4-4AB1-AE91-3D0165543914}" name="Satisfactory Progress" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{19202101-9DC4-4AB1-AE91-3D0165543914}" name="Satisfactory Progress" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{B60F6342-2420-4464-9FE1-640027DFFA28}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{82C08185-62B0-49B8-8BF8-A43FAD604047}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{CAD1A98A-74B0-4F1D-ADD6-0C436D5EDB8E}" name="Dependencies"/>
@@ -1381,9 +1415,9 @@
   <autoFilter ref="A65:H71" xr:uid="{94928A84-CEC8-4686-A48A-A106421EFF97}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{122D3763-DD48-4DB8-8D44-5D63ED13E699}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{FCD2BFCD-EF2B-4360-B3AE-7271D88EC80B}" name="Week ending date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{FCD2BFCD-EF2B-4360-B3AE-7271D88EC80B}" name="Week ending date" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{BC0C5139-381F-421E-82A5-8F2665A6D53A}" name="Objective"/>
-    <tableColumn id="8" xr3:uid="{27E0CB91-7760-4BBE-98CF-37C7F0809D4C}" name="Satisfactory Progress" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{27E0CB91-7760-4BBE-98CF-37C7F0809D4C}" name="Satisfactory Progress" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{9BFB9637-598D-41DD-B2F0-A8C74A76ABAE}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{C0CAB8E0-A4F5-4C92-8BC8-BDFAC6FC58B3}" name="Deliverables"/>
     <tableColumn id="6" xr3:uid="{8C5A0E92-FB26-4C7B-B09F-68CCE093EF0B}" name="Dependencies"/>
@@ -1690,25 +1724,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="D88" zoomScale="103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.52734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.41015625" customWidth="1"/>
-    <col min="3" max="3" width="57.41015625" customWidth="1"/>
-    <col min="4" max="4" width="19.64453125" customWidth="1"/>
-    <col min="5" max="5" width="55.64453125" customWidth="1"/>
-    <col min="6" max="6" width="25.87890625" customWidth="1"/>
-    <col min="7" max="7" width="38.41015625" customWidth="1"/>
-    <col min="8" max="8" width="27.76171875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="57.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="7" max="7" width="38.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1734,7 +1768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
@@ -1760,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>51</v>
       </c>
@@ -1786,7 +1820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
@@ -1812,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -1838,7 +1872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -1864,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -1890,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1916,7 +1950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1942,7 +1976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1968,7 +2002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1994,7 +2028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -2020,7 +2054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -2046,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -2072,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +2132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
@@ -2124,7 +2158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -2150,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
@@ -2176,7 +2210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
@@ -2202,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
@@ -2228,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -2254,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2280,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -2306,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
@@ -2332,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -2358,7 +2392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
@@ -2384,7 +2418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
@@ -2410,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
@@ -2436,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2462,7 +2496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
@@ -2488,7 +2522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>51</v>
       </c>
@@ -2514,7 +2548,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>52</v>
       </c>
@@ -2540,7 +2574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>53</v>
       </c>
@@ -2566,7 +2600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>54</v>
       </c>
@@ -2592,7 +2626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
@@ -2618,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2644,7 +2678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>50</v>
       </c>
@@ -2670,7 +2704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>51</v>
       </c>
@@ -2696,7 +2730,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>52</v>
       </c>
@@ -2722,7 +2756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
@@ -2748,7 +2782,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>54</v>
       </c>
@@ -2774,7 +2808,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -2798,7 +2832,7 @@
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2824,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
@@ -2850,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>51</v>
       </c>
@@ -2876,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>52</v>
       </c>
@@ -2902,7 +2936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>53</v>
       </c>
@@ -2928,7 +2962,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
@@ -2954,7 +2988,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
@@ -2980,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -3006,7 +3040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>50</v>
       </c>
@@ -3032,7 +3066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>51</v>
       </c>
@@ -3058,7 +3092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>52</v>
       </c>
@@ -3084,7 +3118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>53</v>
       </c>
@@ -3110,7 +3144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
@@ -3136,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
@@ -3162,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -3188,7 +3222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>50</v>
       </c>
@@ -3214,7 +3248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>51</v>
       </c>
@@ -3240,7 +3274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>52</v>
       </c>
@@ -3266,7 +3300,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>53</v>
       </c>
@@ -3292,7 +3326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>54</v>
       </c>
@@ -3318,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>55</v>
       </c>
@@ -3344,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -3370,7 +3404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>50</v>
       </c>
@@ -3396,7 +3430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>51</v>
       </c>
@@ -3422,7 +3456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>52</v>
       </c>
@@ -3448,7 +3482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>53</v>
       </c>
@@ -3474,7 +3508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>54</v>
       </c>
@@ -3500,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>55</v>
       </c>
@@ -3526,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -3552,7 +3586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>50</v>
       </c>
@@ -3578,7 +3612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>51</v>
       </c>
@@ -3604,7 +3638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>52</v>
       </c>
@@ -3630,7 +3664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>53</v>
       </c>
@@ -3656,7 +3690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>54</v>
       </c>
@@ -3682,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>55</v>
       </c>
@@ -3708,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -3734,7 +3768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>50</v>
       </c>
@@ -3760,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>51</v>
       </c>
@@ -3786,7 +3820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>52</v>
       </c>
@@ -3812,7 +3846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>53</v>
       </c>
@@ -3838,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>54</v>
       </c>
@@ -3864,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>55</v>
       </c>
@@ -3890,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -3916,7 +3950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>50</v>
       </c>
@@ -3942,7 +3976,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>51</v>
       </c>
@@ -3968,7 +4002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>52</v>
       </c>
@@ -3994,7 +4028,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>53</v>
       </c>
@@ -4020,7 +4054,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>54</v>
       </c>
@@ -4046,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>55</v>
       </c>
@@ -4072,7 +4106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -4098,7 +4132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -4118,7 +4152,7 @@
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>51</v>
       </c>
@@ -4140,7 +4174,7 @@
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>52</v>
       </c>
@@ -4166,7 +4200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>53</v>
       </c>
@@ -4186,7 +4220,7 @@
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>54</v>
       </c>
@@ -4212,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>55</v>
       </c>
@@ -4235,6 +4269,172 @@
         <v>12</v>
       </c>
       <c r="H111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>3</v>
+      </c>
+      <c r="E113" t="s">
+        <v>4</v>
+      </c>
+      <c r="F113" t="s">
+        <v>5</v>
+      </c>
+      <c r="G113" t="s">
+        <v>6</v>
+      </c>
+      <c r="H113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>50</v>
+      </c>
+      <c r="B114" s="6"/>
+      <c r="C114" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>51</v>
+      </c>
+      <c r="B115" s="6">
+        <v>43895</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B116" s="4">
+        <v>43902</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H116" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>53</v>
+      </c>
+      <c r="B117" s="6"/>
+      <c r="C117" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B118" s="2">
+        <v>43888</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B119" s="2">
+        <v>43888</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H119" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4251,7 +4451,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
-  <tableParts count="14">
+  <tableParts count="15">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -4266,6 +4466,7 @@
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>